<commit_message>
Remove files and materials modification
</commit_message>
<xml_diff>
--- a/Materials/Material.xlsx
+++ b/Materials/Material.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fakiko\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Documents\GitHub\OPEN-UMA-Rover\Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{36897E87-D59C-423A-B04A-3C49FB364BBC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
   <si>
     <t>LM18200T</t>
   </si>
@@ -112,12 +111,18 @@
   </si>
   <si>
     <t>https://www.sparkfun.com/products/13750</t>
+  </si>
+  <si>
+    <t>Raspberry PI 3 B+</t>
+  </si>
+  <si>
+    <t>https://es.farnell.com/raspberry-pi/rpi3-modbp/ordenador-monoplaca-raspberry/dp/2842228</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -174,8 +179,36 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -449,23 +482,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="90.5546875" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="90.5703125" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -482,7 +515,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -494,7 +527,7 @@
         <v>247.64</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -510,7 +543,7 @@
         <v>69.44</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -522,7 +555,7 @@
         <v>16.95</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -534,7 +567,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -546,7 +579,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -558,7 +591,7 @@
         <v>1.06</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -570,7 +603,7 @@
         <v>48.99</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -584,7 +617,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -598,7 +631,7 @@
         <v>0.75</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -613,7 +646,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -628,7 +661,7 @@
         <v>0.78</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
@@ -643,7 +676,7 @@
         <v>31.16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
@@ -658,7 +691,7 @@
         <v>8.18</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -672,7 +705,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -687,7 +720,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -702,7 +735,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -717,7 +750,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>14</v>
       </c>
@@ -732,7 +765,7 @@
       </c>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>4</v>
       </c>
@@ -748,25 +781,44 @@
       </c>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D21" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="2">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2842228</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21">
+        <v>32.46</v>
+      </c>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
         <v>5</v>
       </c>
-      <c r="E21">
-        <f>SUM(E2:E20)</f>
-        <v>482.7</v>
-      </c>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.3">
-      <c r="N35" t="s">
+      <c r="E22">
+        <f>SUM(E2:E21)</f>
+        <v>515.16</v>
+      </c>
+    </row>
+    <row r="36" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N36" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{7FA98D88-E6A2-403A-95A6-186A08F567AD}"/>
-    <hyperlink ref="D20" r:id="rId2" xr:uid="{A64A3B5C-81F6-4F00-9CF6-EB71341D2536}"/>
+    <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D20" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>